<commit_message>
Cambios acerca de la lógica de los atribos en el enriquecido de conjuntos residenciales PENDIENTE: Revisar la posibilidad de añadir una entidad día para limitar los turnos por día
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelo De Dominio Enriquecido Gestión de conjuntos residenciales.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelo De Dominio Enriquecido Gestión de conjuntos residenciales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848FBA12-409E-4E81-9124-80C57BAF0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{848FBA12-409E-4E81-9124-80C57BAF0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22BF6FFE-A7C4-49BD-86EA-AE2E9277428F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -2621,7 +2621,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="153">
   <si>
     <t>Tipo Objeto Dominio</t>
   </si>
@@ -3047,6 +3047,39 @@
   </si>
   <si>
     <t>Objeto de dominio que representa a cada uno de los conjuntos residenciales existentes.</t>
+  </si>
+  <si>
+    <t>disponibilidad</t>
+  </si>
+  <si>
+    <t>Sólo un valor logico con formato SI/NO</t>
+  </si>
+  <si>
+    <t>Representa la disponibilidad de una zona común.</t>
+  </si>
+  <si>
+    <t>DD/MM/AAAA dónde DD representa el día, MM representa el mes, y AAAA representa el año</t>
+  </si>
+  <si>
+    <t>Representa el día en el que está asociado el turno.</t>
+  </si>
+  <si>
+    <t>disponibilidadPersonas</t>
+  </si>
+  <si>
+    <t>Sólo un número entero.</t>
+  </si>
+  <si>
+    <t>Representa la cantidad de cupos que hay disponibles para un mismo turno.</t>
+  </si>
+  <si>
+    <t>Sólo un valor lógico.</t>
+  </si>
+  <si>
+    <t>turnoReservable</t>
+  </si>
+  <si>
+    <t>Representa si el turno puede ser reservado.</t>
   </si>
 </sst>
 </file>
@@ -3473,7 +3506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3662,6 +3695,48 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3695,15 +3770,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3716,42 +3785,6 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3772,6 +3805,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4197,19 +4236,19 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="60"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4217,7 +4256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4225,7 +4264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -4233,52 +4272,52 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -4299,7 +4338,7 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4310,20 +4349,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691F8BFD-AB91-4BB3-AD21-0479D3D78DFA}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -4333,7 +4372,7 @@
       <c r="C1" s="61"/>
       <c r="D1" s="62"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
@@ -4347,7 +4386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
@@ -4362,7 +4401,7 @@
         <v>Gestión de conjuntos residenciales</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
@@ -4374,7 +4413,7 @@
       </c>
       <c r="D4" s="64"/>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>77</v>
       </c>
@@ -4386,7 +4425,7 @@
       </c>
       <c r="D5" s="64"/>
     </row>
-    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>78</v>
       </c>
@@ -4398,7 +4437,7 @@
       </c>
       <c r="D6" s="64"/>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>79</v>
       </c>
@@ -4410,7 +4449,7 @@
       </c>
       <c r="D7" s="64"/>
     </row>
-    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>80</v>
       </c>
@@ -4447,103 +4486,103 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="85" t="str">
         <f>'Listado Objetos de Dominio'!A3</f>
         <v>ConjuntoResidencial</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="72" t="str">
+      <c r="B3" s="86" t="str">
         <f>'Listado Objetos de Dominio'!B3</f>
         <v>Objeto de dominio que representa a cada uno de los conjuntos residenciales existentes.</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
@@ -4612,7 +4651,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>41</v>
       </c>
@@ -4657,7 +4696,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>46</v>
       </c>
@@ -4704,7 +4743,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>67</v>
       </c>
@@ -4749,7 +4788,7 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>86</v>
       </c>
@@ -4778,7 +4817,7 @@
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>87</v>
       </c>
@@ -4823,15 +4862,15 @@
       <c r="T9" s="30"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
+    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="75"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="88"/>
+      <c r="C11" s="89"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>51</v>
       </c>
@@ -4842,66 +4881,66 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="80" t="s">
+    <row r="13" spans="1:21" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="94" t="s">
         <v>91</v>
       </c>
       <c r="C13" s="57" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81"/>
-      <c r="B14" s="83"/>
+    <row r="14" spans="1:21" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="93"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="57" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77" t="s">
+      <c r="B16" s="74"/>
+      <c r="C16" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77" t="s">
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="77" t="s">
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="77"/>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="77"/>
-      <c r="P16" s="77" t="s">
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="Q16" s="77"/>
-      <c r="R16" s="77" t="s">
+      <c r="Q16" s="74"/>
+      <c r="R16" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="S16" s="84"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
+      <c r="S16" s="75"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="91"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
       <c r="H17" s="36" t="s">
         <v>58</v>
       </c>
@@ -4914,12 +4953,12 @@
       <c r="K17" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="79" t="s">
+      <c r="L17" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
+      <c r="M17" s="76"/>
+      <c r="N17" s="76"/>
+      <c r="O17" s="76"/>
       <c r="P17" s="36" t="s">
         <v>60</v>
       </c>
@@ -4933,93 +4972,93 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="85" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
       <c r="H18" s="14"/>
       <c r="I18" s="12"/>
       <c r="J18" s="13"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
       <c r="S18" s="38"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="66" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
       <c r="H19" s="41"/>
       <c r="I19" s="39"/>
       <c r="J19" s="40"/>
       <c r="K19" s="42"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="83"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="43"/>
       <c r="R19" s="43"/>
       <c r="S19" s="44"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="88" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
       <c r="H20" s="46"/>
       <c r="I20" s="47"/>
       <c r="J20" s="45"/>
       <c r="K20" s="48"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="91"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
       <c r="P20" s="30"/>
       <c r="Q20" s="49"/>
       <c r="R20" s="49"/>
       <c r="S20" s="50"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="92" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
       <c r="H21" s="52"/>
       <c r="I21" s="53"/>
       <c r="J21" s="51"/>
       <c r="K21" s="52"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="95"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="54"/>
       <c r="R21" s="54"/>
@@ -5027,17 +5066,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="L19:O19"/>
@@ -5052,6 +5080,17 @@
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{68C0436B-E79D-44A7-88CE-82BDE933D82F}"/>
@@ -5087,109 +5126,109 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC94481-E3CC-43E3-941E-02D7E4865B6C}">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="85" t="str">
         <f>'[1]Listado Objetos de Dominio'!A5</f>
         <v>Residente</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="72" t="str">
+      <c r="B3" s="86" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
@@ -5242,23 +5281,23 @@
         <v>2</v>
       </c>
       <c r="R4" s="19" t="str">
-        <f>A22</f>
+        <f>A23</f>
         <v>Reponsabilidad 1</v>
       </c>
       <c r="S4" s="20" t="str">
-        <f>A23</f>
+        <f>A24</f>
         <v>Reponsabilidad 2</v>
       </c>
       <c r="T4" s="21" t="str">
-        <f>A24</f>
+        <f>A25</f>
         <v>Reponsabilidad 3</v>
       </c>
       <c r="U4" s="22" t="str">
-        <f>A25</f>
+        <f>A26</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>41</v>
       </c>
@@ -5303,7 +5342,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>46</v>
       </c>
@@ -5350,7 +5389,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>92</v>
       </c>
@@ -5375,7 +5414,7 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>93</v>
       </c>
@@ -5420,7 +5459,7 @@
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>73</v>
       </c>
@@ -5461,12 +5500,12 @@
       <c r="T9" s="30"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -5474,8 +5513,8 @@
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
-      <c r="I10" s="25" t="s">
-        <v>140</v>
+      <c r="I10" s="24" t="s">
+        <v>143</v>
       </c>
       <c r="J10" s="24"/>
       <c r="K10" s="26"/>
@@ -5495,16 +5534,16 @@
         <v>44</v>
       </c>
       <c r="Q10" s="25" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="R10" s="28"/>
       <c r="S10" s="29"/>
       <c r="T10" s="30"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:21" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>12</v>
@@ -5536,32 +5575,28 @@
         <v>44</v>
       </c>
       <c r="Q11" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R11" s="28"/>
       <c r="S11" s="29"/>
       <c r="T11" s="30"/>
       <c r="U11" s="31"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="24">
-        <v>1</v>
-      </c>
-      <c r="D12" s="24">
-        <v>130</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
-      <c r="I12" s="24" t="s">
-        <v>68</v>
+      <c r="I12" s="25" t="s">
+        <v>140</v>
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="26"/>
@@ -5581,286 +5616,331 @@
         <v>44</v>
       </c>
       <c r="Q12" s="25" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="R12" s="28"/>
       <c r="S12" s="29"/>
       <c r="T12" s="30"/>
       <c r="U12" s="31"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="24">
+        <v>1</v>
+      </c>
+      <c r="D13" s="24">
+        <v>130</v>
+      </c>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="I13" s="24" t="s">
+        <v>68</v>
+      </c>
       <c r="J13" s="24"/>
       <c r="K13" s="26"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="25"/>
+      <c r="L13" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N13" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O13" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P13" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q13" s="25" t="s">
+        <v>69</v>
+      </c>
       <c r="R13" s="28"/>
       <c r="S13" s="29"/>
       <c r="T13" s="30"/>
       <c r="U13" s="31"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="56"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="96" t="s">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="31"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="56"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="97"/>
-      <c r="C15" s="98"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="B16" s="97"/>
+      <c r="C16" s="98"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B17" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C17" s="34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="34.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="80" t="s">
+    <row r="18" spans="1:19" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B18" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C18" s="35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="81"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="35" t="s">
+    <row r="19" spans="1:19" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="93"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
+    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77" t="s">
+      <c r="B21" s="74"/>
+      <c r="C21" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77" t="s">
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="77"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="77" t="s">
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="L20" s="77"/>
-      <c r="M20" s="77"/>
-      <c r="N20" s="77"/>
-      <c r="O20" s="77"/>
-      <c r="P20" s="77" t="s">
+      <c r="L21" s="74"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="74"/>
+      <c r="O21" s="74"/>
+      <c r="P21" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="Q20" s="77"/>
-      <c r="R20" s="77" t="s">
+      <c r="Q21" s="74"/>
+      <c r="R21" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="S20" s="84"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="78"/>
-      <c r="B21" s="79"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="36" t="s">
+      <c r="S21" s="75"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="91"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="I21" s="36" t="s">
+      <c r="I22" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="36" t="s">
+      <c r="J22" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K21" s="36" t="s">
+      <c r="K22" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L21" s="79" t="s">
+      <c r="L22" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="36" t="s">
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="76"/>
+      <c r="P22" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="Q21" s="36" t="s">
+      <c r="Q22" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="R21" s="36" t="s">
+      <c r="R22" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="S21" s="37" t="s">
+      <c r="S22" s="37" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="85" t="s">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="86"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="87"/>
-      <c r="N22" s="87"/>
-      <c r="O22" s="87"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="38"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="66" t="s">
+      <c r="B23" s="78"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="79"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="38"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="67"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="69"/>
-      <c r="O23" s="69"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="44"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="88" t="s">
+      <c r="B24" s="81"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="83"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="44"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="91"/>
-      <c r="M24" s="91"/>
-      <c r="N24" s="91"/>
-      <c r="O24" s="91"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="49"/>
-      <c r="S24" s="50"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="92" t="s">
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="69"/>
+      <c r="N25" s="69"/>
+      <c r="O25" s="69"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="50"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="93"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="95"/>
-      <c r="N25" s="95"/>
-      <c r="O25" s="95"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="55"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="73"/>
+      <c r="O26" s="73"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="L22:O22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="L23:O23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="L24:O24"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:G22"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B8FCC087-AC99-4C6B-BC9A-E2AC36CAED41}"/>
-    <hyperlink ref="I25" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{CDF51FA1-95E8-458D-B08D-DE6B83D11E90}"/>
+    <hyperlink ref="I26" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{CDF51FA1-95E8-458D-B08D-DE6B83D11E90}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{E8AED8A1-D46F-4E6A-A688-B030C913C178}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{5204543D-2FD3-4C52-A214-40DAFC4AB330}"/>
     <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{24B0CFBA-B422-4BB7-8C7F-510DDC30BE26}"/>
-    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C597EA1C-A221-4684-B293-242B3F8A541E}"/>
-    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{56C317F9-9561-44AC-B9C2-329CFDD0A0FD}"/>
-    <hyperlink ref="A25:B25" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{D41B6581-A976-442C-B954-5594B5BDBAE4}"/>
+    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C597EA1C-A221-4684-B293-242B3F8A541E}"/>
+    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{56C317F9-9561-44AC-B9C2-329CFDD0A0FD}"/>
+    <hyperlink ref="A26:B26" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{D41B6581-A976-442C-B954-5594B5BDBAE4}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{307E0460-9076-4914-963A-10FAC8B6A64E}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{E29D6D57-D115-4134-897D-1A336068BAFD}"/>
-    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{832DA90C-BACA-4EC2-B66D-D2764CD09DA1}"/>
-    <hyperlink ref="C18" location="ZonaComun!A6" display="nombre" xr:uid="{80372D6B-38D9-46D9-A913-E7AC275EFEAE}"/>
-    <hyperlink ref="C17" location="ZonaComun!A5" display="identificador" xr:uid="{32D763C1-3B96-49B2-B291-41023CC5DF4A}"/>
+    <hyperlink ref="A25:B25" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{832DA90C-BACA-4EC2-B66D-D2764CD09DA1}"/>
+    <hyperlink ref="C19" location="ZonaComun!A6" display="nombre" xr:uid="{80372D6B-38D9-46D9-A913-E7AC275EFEAE}"/>
+    <hyperlink ref="C18" location="ZonaComun!A5" display="identificador" xr:uid="{32D763C1-3B96-49B2-B291-41023CC5DF4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5871,7 +5951,7 @@
           <x14:formula1>
             <xm:f>Valores!$A$7:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B12</xm:sqref>
+          <xm:sqref>B5:B13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5883,106 +5963,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6705B14E-4108-425C-84CE-31A47173C10C}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView topLeftCell="P2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:Q7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="72" t="str">
+      <c r="B3" s="86" t="str">
         <f>'Listado Objetos de Dominio'!B6</f>
         <v>Objeto de dominio que representa la Agenda programada de manera especifica para cada zona comun.</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
@@ -6051,7 +6131,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>41</v>
       </c>
@@ -6096,7 +6176,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>46</v>
       </c>
@@ -6143,7 +6223,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>101</v>
       </c>
@@ -6156,9 +6236,7 @@
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="25" t="s">
-        <v>140</v>
-      </c>
+      <c r="I7" s="103"/>
       <c r="J7" s="24"/>
       <c r="K7" s="26"/>
       <c r="L7" s="24" t="s">
@@ -6184,7 +6262,7 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>102</v>
       </c>
@@ -6211,17 +6289,17 @@
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="56"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="96" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="97"/>
       <c r="C10" s="98"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>51</v>
       </c>
@@ -6232,66 +6310,66 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="34.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="80" t="s">
+    <row r="12" spans="1:21" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="94" t="s">
         <v>100</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="81"/>
-      <c r="B13" s="83"/>
+    <row r="13" spans="1:21" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="93"/>
+      <c r="B13" s="95"/>
       <c r="C13" s="35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
+    <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77" t="s">
+      <c r="B15" s="74"/>
+      <c r="C15" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77" t="s">
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77" t="s">
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="77"/>
-      <c r="M15" s="77"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="77" t="s">
+      <c r="L15" s="74"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="Q15" s="77"/>
-      <c r="R15" s="77" t="s">
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="S15" s="84"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
+      <c r="S15" s="75"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="91"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
       <c r="H16" s="36" t="s">
         <v>58</v>
       </c>
@@ -6304,12 +6382,12 @@
       <c r="K16" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="79" t="s">
+      <c r="L16" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="M16" s="79"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="76"/>
+      <c r="O16" s="76"/>
       <c r="P16" s="36" t="s">
         <v>60</v>
       </c>
@@ -6323,93 +6401,93 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="85" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="86"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
       <c r="H17" s="14"/>
       <c r="I17" s="12"/>
       <c r="J17" s="13"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
-      <c r="O17" s="87"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="79"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="S17" s="38"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
       <c r="H18" s="41"/>
       <c r="I18" s="39"/>
       <c r="J18" s="40"/>
       <c r="K18" s="42"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="83"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="43"/>
       <c r="R18" s="43"/>
       <c r="S18" s="44"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="88" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="90"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
       <c r="H19" s="46"/>
       <c r="I19" s="47"/>
       <c r="J19" s="45"/>
       <c r="K19" s="48"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="91"/>
-      <c r="N19" s="91"/>
-      <c r="O19" s="91"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
       <c r="P19" s="30"/>
       <c r="Q19" s="49"/>
       <c r="R19" s="49"/>
       <c r="S19" s="50"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="92" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="93"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="94"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
       <c r="H20" s="52"/>
       <c r="I20" s="53"/>
       <c r="J20" s="51"/>
       <c r="K20" s="52"/>
-      <c r="L20" s="95"/>
-      <c r="M20" s="95"/>
-      <c r="N20" s="95"/>
-      <c r="O20" s="95"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
       <c r="P20" s="31"/>
       <c r="Q20" s="54"/>
       <c r="R20" s="54"/>
@@ -6417,18 +6495,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
     <mergeCell ref="R15:S15"/>
     <mergeCell ref="L16:O16"/>
     <mergeCell ref="A1:Q1"/>
@@ -6442,6 +6508,18 @@
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="K15:O15"/>
     <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="L20:O20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{14522053-DD99-446C-9513-67358B768F41}"/>
@@ -6480,106 +6558,106 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="85" t="str">
         <f>'Listado Objetos de Dominio'!A5</f>
         <v>Administrador</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="72" t="str">
+      <c r="B3" s="86" t="str">
         <f>'Listado Objetos de Dominio'!B5</f>
         <v xml:space="preserve"> Objeto de dominio que representa el Administrador encarcador de hacer CRUD a sonas comunes y Usuarios(residentes) , tambien encargado de cancelar reservas.</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
@@ -6648,7 +6726,7 @@
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>41</v>
       </c>
@@ -6693,7 +6771,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>46</v>
       </c>
@@ -6740,7 +6818,7 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>106</v>
       </c>
@@ -6787,7 +6865,7 @@
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>107</v>
       </c>
@@ -6834,7 +6912,7 @@
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>86</v>
       </c>
@@ -6877,7 +6955,7 @@
       <c r="T9" s="30"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>76</v>
       </c>
@@ -6904,17 +6982,17 @@
       <c r="T10" s="30"/>
       <c r="U10" s="31"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="56"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="s">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="75"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="88"/>
+      <c r="C12" s="89"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>51</v>
       </c>
@@ -6925,66 +7003,66 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="94" t="s">
         <v>118</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="100"/>
-      <c r="B15" s="83"/>
+      <c r="B15" s="95"/>
       <c r="C15" s="35" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77" t="s">
+      <c r="B17" s="74"/>
+      <c r="C17" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77" t="s">
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="77" t="s">
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="L17" s="77"/>
-      <c r="M17" s="77"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="77"/>
-      <c r="P17" s="77" t="s">
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="Q17" s="77"/>
-      <c r="R17" s="77" t="s">
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="S17" s="84"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
+      <c r="S17" s="75"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="91"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
       <c r="H18" s="36" t="s">
         <v>58</v>
       </c>
@@ -6997,12 +7075,12 @@
       <c r="K18" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="79" t="s">
+      <c r="L18" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
-      <c r="O18" s="79"/>
+      <c r="M18" s="76"/>
+      <c r="N18" s="76"/>
+      <c r="O18" s="76"/>
       <c r="P18" s="36" t="s">
         <v>60</v>
       </c>
@@ -7016,93 +7094,93 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="85" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
       <c r="H19" s="14"/>
       <c r="I19" s="12"/>
       <c r="J19" s="13"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="87"/>
-      <c r="O19" s="87"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="79"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
       <c r="R19" s="14"/>
       <c r="S19" s="38"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
       <c r="H20" s="41"/>
       <c r="I20" s="39"/>
       <c r="J20" s="40"/>
       <c r="K20" s="42"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="83"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="43"/>
       <c r="R20" s="43"/>
       <c r="S20" s="44"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="88" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="89"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
       <c r="H21" s="46"/>
       <c r="I21" s="47"/>
       <c r="J21" s="45"/>
       <c r="K21" s="48"/>
-      <c r="L21" s="91"/>
-      <c r="M21" s="91"/>
-      <c r="N21" s="91"/>
-      <c r="O21" s="91"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
       <c r="P21" s="30"/>
       <c r="Q21" s="49"/>
       <c r="R21" s="49"/>
       <c r="S21" s="50"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="92" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="94"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
       <c r="H22" s="52"/>
       <c r="I22" s="53"/>
       <c r="J22" s="51"/>
       <c r="K22" s="52"/>
-      <c r="L22" s="95"/>
-      <c r="M22" s="95"/>
-      <c r="N22" s="95"/>
-      <c r="O22" s="95"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="73"/>
       <c r="P22" s="31"/>
       <c r="Q22" s="54"/>
       <c r="R22" s="54"/>
@@ -7110,6 +7188,17 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="L19:O19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="L20:O20"/>
@@ -7124,17 +7213,6 @@
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{0E7B0C62-6DE1-4F39-948B-B7E7FB6516CF}"/>
@@ -7171,109 +7249,109 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B4121A-D579-436D-BD34-A6CF989D3F28}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="85" t="str">
         <f>'Listado Objetos de Dominio'!A7</f>
         <v>Turno</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="72" t="str">
+      <c r="B3" s="86" t="str">
         <f>'Listado Objetos de Dominio'!B7</f>
         <v>Objeto de dominio que representa a cada Turno que esta programado con respecto al tiempo de uso según la zona comun y con respecto a la agenda disponible.</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
@@ -7326,23 +7404,23 @@
         <v>2</v>
       </c>
       <c r="R4" s="19" t="str">
-        <f>A18</f>
+        <f>A21</f>
         <v>Reponsabilidad 1</v>
       </c>
       <c r="S4" s="20" t="str">
-        <f>A19</f>
+        <f>A22</f>
         <v>Reponsabilidad 2</v>
       </c>
       <c r="T4" s="21" t="str">
-        <f>A20</f>
+        <f>A23</f>
         <v>Reponsabilidad 3</v>
       </c>
       <c r="U4" s="22" t="str">
-        <f>A21</f>
+        <f>A24</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>41</v>
       </c>
@@ -7387,7 +7465,7 @@
       <c r="T5" s="30"/>
       <c r="U5" s="31"/>
     </row>
-    <row r="6" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>119</v>
       </c>
@@ -7412,7 +7490,7 @@
         <v>123</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M6" s="24" t="s">
         <v>44</v>
@@ -7434,12 +7512,12 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -7447,12 +7525,12 @@
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="25" t="s">
-        <v>140</v>
+      <c r="I7" s="104" t="s">
+        <v>145</v>
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="27" t="s">
         <v>44</v>
       </c>
       <c r="M7" s="24" t="s">
@@ -7468,16 +7546,16 @@
         <v>44</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="R7" s="28"/>
       <c r="S7" s="29"/>
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>12</v>
@@ -7509,19 +7587,790 @@
         <v>44</v>
       </c>
       <c r="Q8" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="R8" s="28"/>
       <c r="S8" s="29"/>
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="R9" s="28"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="31"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="24">
+        <v>1</v>
+      </c>
+      <c r="D10" s="24">
+        <v>200</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P10" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q10" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="R10" s="28"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="31"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q11" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="R11" s="28"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="31"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
         <v>124</v>
       </c>
+      <c r="B12" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="31"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="56"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="87" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="99" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="100"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="90" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="74"/>
+      <c r="C19" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="L19" s="74"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="74"/>
+      <c r="P19" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q19" s="74"/>
+      <c r="R19" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="S19" s="75"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="91"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="76"/>
+      <c r="P20" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q20" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="S20" s="37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="78"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="79"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="38"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="81"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="44"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="67"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="69"/>
+      <c r="O23" s="69"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="50"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="71"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="73"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{87E5FC51-2E20-487C-809E-702D72E38ACE}"/>
+    <hyperlink ref="I24" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{9A04E92F-1529-4FD3-8E93-A1013850ECEB}"/>
+    <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{BE5BBDEB-D136-4A69-B76E-B9EE18B4AADF}"/>
+    <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{D01A25A8-47B1-4A34-B537-75FC9B240CD7}"/>
+    <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{92F40FB2-A95D-48A6-9D44-842275D8A002}"/>
+    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C0E8065D-3D44-47C0-B62D-9C1975E78394}"/>
+    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{87B8DA9D-DFC9-46D8-BA58-B9DFB0075785}"/>
+    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{5FAE9D83-2CFB-4516-8C0E-0483F9E7D414}"/>
+    <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{CDA72146-A8A4-4D15-95BA-54212217969C}"/>
+    <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{FA8306A6-9560-44AE-8D58-CD1ED4D8F35F}"/>
+    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{5ABA868F-0891-4351-9AEE-F3E42FC356A3}"/>
+    <hyperlink ref="C17" location="TipoZonaComun!A5" display="identificador" xr:uid="{E10B65B9-BDA7-4627-9804-7F151D49B328}"/>
+    <hyperlink ref="C16" location="TipoZonaComun!A5" display="identificador" xr:uid="{031EE333-7435-4C47-B98E-7785412C28EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{696233DD-873D-4B81-B95F-D4FF24B22192}">
+          <x14:formula1>
+            <xm:f>Valores!$A$7:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:B11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B28FCEC-48B2-4101-A999-B6D0BE7ECE06}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView topLeftCell="I3" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="85" t="str">
+        <f>'Listado Objetos de Dominio'!A8</f>
+        <v>Publicación</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="86" t="str">
+        <f>'Listado Objetos de Dominio'!B8</f>
+        <v xml:space="preserve"> Objeto de dominio que representa el medio de comunicación que hay frente de publicar alguna eventualidad.</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="19" t="str">
+        <f>A18</f>
+        <v>Reponsabilidad 1</v>
+      </c>
+      <c r="S4" s="20" t="str">
+        <f>A19</f>
+        <v>Reponsabilidad 2</v>
+      </c>
+      <c r="T4" s="21" t="str">
+        <f>A20</f>
+        <v>Reponsabilidad 3</v>
+      </c>
+      <c r="U4" s="22" t="str">
+        <f>A21</f>
+        <v>Reponsabilidad 4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="24">
+        <v>32</v>
+      </c>
+      <c r="D5" s="24">
+        <v>32</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="24"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="R5" s="28"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="31"/>
+    </row>
+    <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="24">
+        <v>1</v>
+      </c>
+      <c r="D6" s="24">
+        <v>50</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" s="24"/>
+      <c r="K6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="R6" s="28"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="31"/>
+    </row>
+    <row r="7" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>10000</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="R7" s="28"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="31"/>
+    </row>
+    <row r="8" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="R8" s="28"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="31"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>134</v>
+      </c>
       <c r="B9" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
@@ -7543,17 +8392,17 @@
       <c r="T9" s="30"/>
       <c r="U9" s="31"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="56"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="75"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="88"/>
+      <c r="C11" s="89"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>51</v>
       </c>
@@ -7564,66 +8413,64 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="99" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" s="82" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="94" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="101" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="100"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="35" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
+      <c r="B14" s="95"/>
+      <c r="C14" s="102"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77" t="s">
+      <c r="B16" s="74"/>
+      <c r="C16" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77" t="s">
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="77" t="s">
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="77"/>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="77"/>
-      <c r="P16" s="77" t="s">
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="Q16" s="77"/>
-      <c r="R16" s="77" t="s">
+      <c r="Q16" s="74"/>
+      <c r="R16" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="S16" s="84"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
+      <c r="S16" s="75"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="91"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
       <c r="H17" s="36" t="s">
         <v>58</v>
       </c>
@@ -7636,12 +8483,12 @@
       <c r="K17" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="79" t="s">
+      <c r="L17" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
+      <c r="M17" s="76"/>
+      <c r="N17" s="76"/>
+      <c r="O17" s="76"/>
       <c r="P17" s="36" t="s">
         <v>60</v>
       </c>
@@ -7655,100 +8502,110 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="85" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
       <c r="H18" s="14"/>
       <c r="I18" s="12"/>
       <c r="J18" s="13"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
       <c r="S18" s="38"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="66" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
       <c r="H19" s="41"/>
       <c r="I19" s="39"/>
       <c r="J19" s="40"/>
       <c r="K19" s="42"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="83"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="43"/>
       <c r="R19" s="43"/>
       <c r="S19" s="44"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="88" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
       <c r="H20" s="46"/>
       <c r="I20" s="47"/>
       <c r="J20" s="45"/>
       <c r="K20" s="48"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="91"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
       <c r="P20" s="30"/>
       <c r="Q20" s="49"/>
       <c r="R20" s="49"/>
       <c r="S20" s="50"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="92" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
       <c r="H21" s="52"/>
       <c r="I21" s="53"/>
       <c r="J21" s="51"/>
       <c r="K21" s="52"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="95"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="54"/>
       <c r="R21" s="54"/>
       <c r="S21" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="L17:O17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:G18"/>
@@ -7765,654 +8622,6 @@
     <mergeCell ref="L19:O19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="B13:B14"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{87E5FC51-2E20-487C-809E-702D72E38ACE}"/>
-    <hyperlink ref="I21" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{9A04E92F-1529-4FD3-8E93-A1013850ECEB}"/>
-    <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{BE5BBDEB-D136-4A69-B76E-B9EE18B4AADF}"/>
-    <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{D01A25A8-47B1-4A34-B537-75FC9B240CD7}"/>
-    <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{92F40FB2-A95D-48A6-9D44-842275D8A002}"/>
-    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C0E8065D-3D44-47C0-B62D-9C1975E78394}"/>
-    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{87B8DA9D-DFC9-46D8-BA58-B9DFB0075785}"/>
-    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{5FAE9D83-2CFB-4516-8C0E-0483F9E7D414}"/>
-    <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{CDA72146-A8A4-4D15-95BA-54212217969C}"/>
-    <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{FA8306A6-9560-44AE-8D58-CD1ED4D8F35F}"/>
-    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{5ABA868F-0891-4351-9AEE-F3E42FC356A3}"/>
-    <hyperlink ref="C14" location="TipoZonaComun!A5" display="identificador" xr:uid="{E10B65B9-BDA7-4627-9804-7F151D49B328}"/>
-    <hyperlink ref="C13" location="TipoZonaComun!A5" display="identificador" xr:uid="{031EE333-7435-4C47-B98E-7785412C28EE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{696233DD-873D-4B81-B95F-D4FF24B22192}">
-          <x14:formula1>
-            <xm:f>Valores!$A$7:$A$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5:B8</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B28FCEC-48B2-4101-A999-B6D0BE7ECE06}">
-  <dimension ref="A1:U21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="79.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="71" t="str">
-        <f>'Listado Objetos de Dominio'!A8</f>
-        <v>Publicación</v>
-      </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="72" t="str">
-        <f>'Listado Objetos de Dominio'!B8</f>
-        <v xml:space="preserve"> Objeto de dominio que representa el medio de comunicación que hay frente de publicar alguna eventualidad.</v>
-      </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="R4" s="19" t="str">
-        <f>A18</f>
-        <v>Reponsabilidad 1</v>
-      </c>
-      <c r="S4" s="20" t="str">
-        <f>A19</f>
-        <v>Reponsabilidad 2</v>
-      </c>
-      <c r="T4" s="21" t="str">
-        <f>A20</f>
-        <v>Reponsabilidad 3</v>
-      </c>
-      <c r="U4" s="22" t="str">
-        <f>A21</f>
-        <v>Reponsabilidad 4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="24">
-        <v>32</v>
-      </c>
-      <c r="D5" s="24">
-        <v>32</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="O5" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="P5" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q5" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="R5" s="28"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="31"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="24">
-        <v>1</v>
-      </c>
-      <c r="D6" s="24">
-        <v>50</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="R6" s="28"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="31"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="24">
-        <v>1</v>
-      </c>
-      <c r="D7" s="24">
-        <v>500</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="M7" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="O7" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="R7" s="28"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="31"/>
-    </row>
-    <row r="8" spans="1:21" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="M8" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="N8" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q8" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="R8" s="28"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="31"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="31"/>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="56"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="75"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="99" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="82" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="101" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="102"/>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" s="77"/>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="77"/>
-      <c r="P16" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q16" s="77"/>
-      <c r="R16" s="77" t="s">
-        <v>57</v>
-      </c>
-      <c r="S16" s="84"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="79" t="s">
-        <v>2</v>
-      </c>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q17" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="R17" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="S17" s="37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="38"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="43"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="44"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="88" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="91"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
-      <c r="S20" s="50"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="92" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="95"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="55"/>
-    </row>
-  </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="C16:G17"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:O16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="L19:O19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{928D26AE-809F-43A3-A6BF-D75E5E6D66DA}"/>

</xml_diff>

<commit_message>
primer event sortming de conjuntos residenciales, falta terminarlo, y cambios en los enriquecidos del mismo contexto para los atributos
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelo De Dominio Enriquecido Gestión de conjuntos residenciales.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelo De Dominio Enriquecido Gestión de conjuntos residenciales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{848FBA12-409E-4E81-9124-80C57BAF0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22BF6FFE-A7C4-49BD-86EA-AE2E9277428F}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{848FBA12-409E-4E81-9124-80C57BAF0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5923675-001F-492F-8398-5F9CD0033B6D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="7" xr2:uid="{E5C52C5A-EABC-49E4-B2DE-F2A1DBC4ED29}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -2621,7 +2621,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="160">
   <si>
     <t>Tipo Objeto Dominio</t>
   </si>
@@ -3052,18 +3052,9 @@
     <t>disponibilidad</t>
   </si>
   <si>
-    <t>Sólo un valor logico con formato SI/NO</t>
-  </si>
-  <si>
-    <t>Representa la disponibilidad de una zona común.</t>
-  </si>
-  <si>
     <t>DD/MM/AAAA dónde DD representa el día, MM representa el mes, y AAAA representa el año</t>
   </si>
   <si>
-    <t>Representa el día en el que está asociado el turno.</t>
-  </si>
-  <si>
     <t>disponibilidadPersonas</t>
   </si>
   <si>
@@ -3080,6 +3071,36 @@
   </si>
   <si>
     <t>Representa si el turno puede ser reservado.</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>Representa la fecha en la cual está programada una agenda.</t>
+  </si>
+  <si>
+    <t>Sólo un valor lógico SI/NO</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Representa la disponibilidad de una agenda para ser reservada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un día de la semana, por ejemplo; "Lunes", "Martes" </t>
+  </si>
+  <si>
+    <t>tiempoUsoDia</t>
+  </si>
+  <si>
+    <t>Representa el tiempo de uso que puede darle un residente a una zona común.</t>
+  </si>
+  <si>
+    <t>Representa la agenda a la que está asociada el turno.</t>
+  </si>
+  <si>
+    <t>nombreDeTurno</t>
   </si>
 </sst>
 </file>
@@ -3506,7 +3527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3674,6 +3695,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3805,12 +3835,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4243,10 +4267,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
+      <c r="B1" s="63"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -4366,11 +4390,11 @@
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="65"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -4396,7 +4420,7 @@
       <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="63" t="str">
+      <c r="D3" s="66" t="str">
         <f>$B$1</f>
         <v>Gestión de conjuntos residenciales</v>
       </c>
@@ -4411,7 +4435,7 @@
       <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="64"/>
+      <c r="D4" s="67"/>
     </row>
     <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
@@ -4423,7 +4447,7 @@
       <c r="C5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="64"/>
+      <c r="D5" s="67"/>
     </row>
     <row r="6" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -4435,7 +4459,7 @@
       <c r="C6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="64"/>
+      <c r="D6" s="67"/>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -4447,7 +4471,7 @@
       <c r="C7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="64"/>
+      <c r="D7" s="67"/>
     </row>
     <row r="8" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
@@ -4459,7 +4483,7 @@
       <c r="C8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="65"/>
+      <c r="D8" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4514,73 +4538,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="85" t="str">
+      <c r="B2" s="88" t="str">
         <f>'Listado Objetos de Dominio'!A3</f>
         <v>ConjuntoResidencial</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="86" t="str">
+      <c r="B3" s="89" t="str">
         <f>'Listado Objetos de Dominio'!B3</f>
         <v>Objeto de dominio que representa a cada uno de los conjuntos residenciales existentes.</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -4864,11 +4888,11 @@
     </row>
     <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="89"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
@@ -4882,10 +4906,10 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="95" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="97" t="s">
         <v>91</v>
       </c>
       <c r="C13" s="57" t="s">
@@ -4893,54 +4917,54 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="93"/>
-      <c r="B14" s="95"/>
+      <c r="A14" s="96"/>
+      <c r="B14" s="98"/>
       <c r="C14" s="57" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74" t="s">
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74" t="s">
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74" t="s">
+      <c r="L16" s="77"/>
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74" t="s">
+      <c r="Q16" s="77"/>
+      <c r="R16" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="S16" s="75"/>
+      <c r="S16" s="78"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="91"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
       <c r="H17" s="36" t="s">
         <v>58</v>
       </c>
@@ -4953,12 +4977,12 @@
       <c r="K17" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="76" t="s">
+      <c r="L17" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="79"/>
       <c r="P17" s="36" t="s">
         <v>60</v>
       </c>
@@ -4973,92 +4997,92 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
       <c r="H18" s="14"/>
       <c r="I18" s="12"/>
       <c r="J18" s="13"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="79"/>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
-      <c r="O18" s="79"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="82"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
       <c r="S18" s="38"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
       <c r="H19" s="41"/>
       <c r="I19" s="39"/>
       <c r="J19" s="40"/>
       <c r="K19" s="42"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="83"/>
-      <c r="O19" s="83"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="86"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="43"/>
       <c r="R19" s="43"/>
       <c r="S19" s="44"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="46"/>
       <c r="I20" s="47"/>
       <c r="J20" s="45"/>
       <c r="K20" s="48"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
+      <c r="N20" s="72"/>
+      <c r="O20" s="72"/>
       <c r="P20" s="30"/>
       <c r="Q20" s="49"/>
       <c r="R20" s="49"/>
       <c r="S20" s="50"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
       <c r="H21" s="52"/>
       <c r="I21" s="53"/>
       <c r="J21" s="51"/>
       <c r="K21" s="52"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="73"/>
-      <c r="O21" s="73"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
+      <c r="O21" s="76"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="54"/>
       <c r="R21" s="54"/>
@@ -5128,8 +5152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC94481-E3CC-43E3-941E-02D7E4865B6C}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5160,73 +5184,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="85" t="str">
+      <c r="B2" s="88" t="str">
         <f>'[1]Listado Objetos de Dominio'!A5</f>
         <v>Residente</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="86" t="str">
+      <c r="B3" s="89" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -5502,10 +5526,10 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -5514,7 +5538,7 @@
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J10" s="24"/>
       <c r="K10" s="26"/>
@@ -5534,7 +5558,7 @@
         <v>44</v>
       </c>
       <c r="Q10" s="25" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="R10" s="28"/>
       <c r="S10" s="29"/>
@@ -5699,11 +5723,11 @@
       <c r="D15" s="56"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="97"/>
-      <c r="C16" s="98"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="101"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
@@ -5717,10 +5741,10 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="92" t="s">
+      <c r="A18" s="95" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="94" t="s">
+      <c r="B18" s="97" t="s">
         <v>100</v>
       </c>
       <c r="C18" s="35" t="s">
@@ -5728,54 +5752,54 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="93"/>
-      <c r="B19" s="95"/>
+      <c r="A19" s="96"/>
+      <c r="B19" s="98"/>
       <c r="C19" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="90" t="s">
+      <c r="A21" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74" t="s">
+      <c r="B21" s="77"/>
+      <c r="C21" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74" t="s">
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74" t="s">
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="74" t="s">
+      <c r="L21" s="77"/>
+      <c r="M21" s="77"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="77"/>
+      <c r="P21" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="Q21" s="74"/>
-      <c r="R21" s="74" t="s">
+      <c r="Q21" s="77"/>
+      <c r="R21" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="S21" s="75"/>
+      <c r="S21" s="78"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="91"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
+      <c r="A22" s="94"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="79"/>
       <c r="H22" s="36" t="s">
         <v>58</v>
       </c>
@@ -5788,12 +5812,12 @@
       <c r="K22" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="76" t="s">
+      <c r="L22" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M22" s="76"/>
-      <c r="N22" s="76"/>
-      <c r="O22" s="76"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
       <c r="P22" s="36" t="s">
         <v>60</v>
       </c>
@@ -5808,92 +5832,92 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
       <c r="H23" s="14"/>
       <c r="I23" s="12"/>
       <c r="J23" s="13"/>
       <c r="K23" s="12"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="79"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="82"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="14"/>
       <c r="S23" s="38"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="80" t="s">
+      <c r="A24" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
       <c r="H24" s="41"/>
       <c r="I24" s="39"/>
       <c r="J24" s="40"/>
       <c r="K24" s="42"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="83"/>
-      <c r="N24" s="83"/>
-      <c r="O24" s="83"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="86"/>
+      <c r="O24" s="86"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="43"/>
       <c r="R24" s="43"/>
       <c r="S24" s="44"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
       <c r="H25" s="46"/>
       <c r="I25" s="47"/>
       <c r="J25" s="45"/>
       <c r="K25" s="48"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="72"/>
       <c r="P25" s="30"/>
       <c r="Q25" s="49"/>
       <c r="R25" s="49"/>
       <c r="S25" s="50"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
       <c r="H26" s="52"/>
       <c r="I26" s="53"/>
       <c r="J26" s="51"/>
       <c r="K26" s="52"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="73"/>
-      <c r="O26" s="73"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="76"/>
+      <c r="O26" s="76"/>
       <c r="P26" s="31"/>
       <c r="Q26" s="54"/>
       <c r="R26" s="54"/>
@@ -5961,10 +5985,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6705B14E-4108-425C-84CE-31A47173C10C}">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5995,72 +6019,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="86" t="str">
+      <c r="B3" s="89" t="str">
         <f>'Listado Objetos de Dominio'!B6</f>
         <v>Objeto de dominio que representa la Agenda programada de manera especifica para cada zona comun.</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -6115,19 +6139,19 @@
         <v>2</v>
       </c>
       <c r="R4" s="19" t="str">
-        <f>A17</f>
+        <f>A19</f>
         <v>Reponsabilidad 1</v>
       </c>
       <c r="S4" s="20" t="str">
-        <f>A18</f>
+        <f>A20</f>
         <v>Reponsabilidad 2</v>
       </c>
       <c r="T4" s="21" t="str">
-        <f>A19</f>
+        <f>A21</f>
         <v>Reponsabilidad 3</v>
       </c>
       <c r="U4" s="22" t="str">
-        <f>A20</f>
+        <f>A22</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
@@ -6225,10 +6249,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -6236,10 +6260,14 @@
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="24"/>
+      <c r="I7" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>153</v>
+      </c>
       <c r="K7" s="26"/>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="27" t="s">
         <v>44</v>
       </c>
       <c r="M7" s="24" t="s">
@@ -6255,19 +6283,19 @@
         <v>44</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="R7" s="28"/>
       <c r="S7" s="29"/>
       <c r="T7" s="30"/>
       <c r="U7" s="31"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -6275,266 +6303,348 @@
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="I8" s="61" t="s">
+        <v>143</v>
+      </c>
       <c r="J8" s="24"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="25"/>
+      <c r="L8" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>151</v>
+      </c>
       <c r="R8" s="28"/>
       <c r="S8" s="29"/>
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="56"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="60" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="R9" s="28"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="31"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="31"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="56"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="97"/>
-      <c r="C10" s="98"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+      <c r="B12" s="100"/>
+      <c r="C12" s="101"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C13" s="34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="92" t="s">
+    <row r="14" spans="1:21" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="95" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="94" t="s">
+      <c r="B14" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C14" s="35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="93"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="35" t="s">
+    <row r="15" spans="1:21" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="96"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="90" t="s">
+    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74" t="s">
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74" t="s">
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="74"/>
-      <c r="M15" s="74"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="74"/>
-      <c r="P15" s="74" t="s">
+      <c r="L17" s="77"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="77"/>
+      <c r="P17" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74" t="s">
+      <c r="Q17" s="77"/>
+      <c r="R17" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="S15" s="75"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="91"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="36" t="s">
+      <c r="S17" s="78"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="94"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I18" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="36" t="s">
+      <c r="J18" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="36" t="s">
+      <c r="K18" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="76" t="s">
+      <c r="L18" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M16" s="76"/>
-      <c r="N16" s="76"/>
-      <c r="O16" s="76"/>
-      <c r="P16" s="36" t="s">
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="Q16" s="36" t="s">
+      <c r="Q18" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="R16" s="36" t="s">
+      <c r="R18" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="S16" s="37" t="s">
+      <c r="S18" s="37" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="77" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="38"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="80" t="s">
+      <c r="B19" s="81"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="38"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="83"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="44"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="B20" s="84"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="86"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+      <c r="S20" s="44"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="49"/>
-      <c r="S19" s="50"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="70" t="s">
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="50"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
-      <c r="N20" s="73"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="54"/>
-      <c r="S20" s="55"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="76"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="L18:O18"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="C15:G16"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:G18"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:O17"/>
+    <mergeCell ref="P17:Q17"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="L19:O19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="L22:O22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{14522053-DD99-446C-9513-67358B768F41}"/>
-    <hyperlink ref="I20" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{C973AD29-00C2-4AC4-BFE3-781984BCA3BC}"/>
+    <hyperlink ref="I22" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{C973AD29-00C2-4AC4-BFE3-781984BCA3BC}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{CBACF441-A6CA-49BD-BBD0-BA64307B60F9}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{825E9808-255E-4C2E-BC7A-C3341AABA37B}"/>
     <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{649FDE9D-5A36-4F11-9B88-2D2E3A9364DD}"/>
-    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C52F8CE6-667C-4433-9617-2292A35632AB}"/>
-    <hyperlink ref="A17:B17" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{02DA2326-010A-4B8B-9633-46C7C8483233}"/>
-    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{B420B7E9-D0A4-4C6F-B6A6-F5FDB8504376}"/>
+    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C52F8CE6-667C-4433-9617-2292A35632AB}"/>
+    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{02DA2326-010A-4B8B-9633-46C7C8483233}"/>
+    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{B420B7E9-D0A4-4C6F-B6A6-F5FDB8504376}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{4F06C042-2484-41EA-BF6C-9D810CB20A2F}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{970855DF-3E15-4A5D-B956-555767FE5676}"/>
-    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{7016E8F1-FB33-43C7-B794-12BDC7300B03}"/>
-    <hyperlink ref="C13" location="Agenda!A6" display="nombre" xr:uid="{6BBEAE49-2A50-4716-BAC9-CE846B53BA22}"/>
-    <hyperlink ref="C12" location="Agenda!A5" display="identificador" xr:uid="{02A2E105-FE7C-4121-9CC2-6176F63127C9}"/>
+    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{7016E8F1-FB33-43C7-B794-12BDC7300B03}"/>
+    <hyperlink ref="C15" location="Agenda!A6" display="nombre" xr:uid="{6BBEAE49-2A50-4716-BAC9-CE846B53BA22}"/>
+    <hyperlink ref="C14" location="Agenda!A5" display="identificador" xr:uid="{02A2E105-FE7C-4121-9CC2-6176F63127C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6545,7 +6655,7 @@
           <x14:formula1>
             <xm:f>Valores!$A$7:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B7</xm:sqref>
+          <xm:sqref>B5:B9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6589,73 +6699,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="85" t="str">
+      <c r="B2" s="88" t="str">
         <f>'Listado Objetos de Dominio'!A5</f>
         <v>Administrador</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="86" t="str">
+      <c r="B3" s="89" t="str">
         <f>'Listado Objetos de Dominio'!B5</f>
         <v xml:space="preserve"> Objeto de dominio que representa el Administrador encarcador de hacer CRUD a sonas comunes y Usuarios(residentes) , tambien encargado de cancelar reservas.</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -6986,11 +7096,11 @@
       <c r="D11" s="56"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="92"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
@@ -7004,10 +7114,10 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="97" t="s">
         <v>118</v>
       </c>
       <c r="C14" s="35" t="s">
@@ -7015,54 +7125,54 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="100"/>
-      <c r="B15" s="95"/>
+      <c r="A15" s="103"/>
+      <c r="B15" s="98"/>
       <c r="C15" s="35" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74" t="s">
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74" t="s">
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74" t="s">
+      <c r="L17" s="77"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="77"/>
+      <c r="P17" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74" t="s">
+      <c r="Q17" s="77"/>
+      <c r="R17" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="S17" s="75"/>
+      <c r="S17" s="78"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="91"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
       <c r="H18" s="36" t="s">
         <v>58</v>
       </c>
@@ -7075,12 +7185,12 @@
       <c r="K18" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="76" t="s">
+      <c r="L18" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
       <c r="P18" s="36" t="s">
         <v>60</v>
       </c>
@@ -7095,92 +7205,92 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
       <c r="H19" s="14"/>
       <c r="I19" s="12"/>
       <c r="J19" s="13"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
       <c r="R19" s="14"/>
       <c r="S19" s="38"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
       <c r="H20" s="41"/>
       <c r="I20" s="39"/>
       <c r="J20" s="40"/>
       <c r="K20" s="42"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="83"/>
-      <c r="O20" s="83"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="86"/>
       <c r="P20" s="29"/>
       <c r="Q20" s="43"/>
       <c r="R20" s="43"/>
       <c r="S20" s="44"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="67"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
       <c r="H21" s="46"/>
       <c r="I21" s="47"/>
       <c r="J21" s="45"/>
       <c r="K21" s="48"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="69"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="72"/>
       <c r="P21" s="30"/>
       <c r="Q21" s="49"/>
       <c r="R21" s="49"/>
       <c r="S21" s="50"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
       <c r="H22" s="52"/>
       <c r="I22" s="53"/>
       <c r="J22" s="51"/>
       <c r="K22" s="52"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
-      <c r="O22" s="73"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="76"/>
       <c r="P22" s="31"/>
       <c r="Q22" s="54"/>
       <c r="R22" s="54"/>
@@ -7249,10 +7359,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B4121A-D579-436D-BD34-A6CF989D3F28}">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7283,73 +7393,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="85" t="str">
+      <c r="B2" s="88" t="str">
         <f>'Listado Objetos de Dominio'!A7</f>
         <v>Turno</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="86" t="str">
+      <c r="B3" s="89" t="str">
         <f>'Listado Objetos de Dominio'!B7</f>
         <v>Objeto de dominio que representa a cada Turno que esta programado con respecto al tiempo de uso según la zona comun y con respecto a la agenda disponible.</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -7404,19 +7514,19 @@
         <v>2</v>
       </c>
       <c r="R4" s="19" t="str">
+        <f>A20</f>
+        <v>Reponsabilidad 1</v>
+      </c>
+      <c r="S4" s="20" t="str">
         <f>A21</f>
-        <v>Reponsabilidad 1</v>
-      </c>
-      <c r="S4" s="20" t="str">
+        <v>Reponsabilidad 2</v>
+      </c>
+      <c r="T4" s="21" t="str">
         <f>A22</f>
-        <v>Reponsabilidad 2</v>
-      </c>
-      <c r="T4" s="21" t="str">
+        <v>Reponsabilidad 3</v>
+      </c>
+      <c r="U4" s="22" t="str">
         <f>A23</f>
-        <v>Reponsabilidad 3</v>
-      </c>
-      <c r="U4" s="22" t="str">
-        <f>A24</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
@@ -7467,7 +7577,7 @@
     </row>
     <row r="6" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>9</v>
@@ -7512,12 +7622,12 @@
       <c r="T6" s="30"/>
       <c r="U6" s="31"/>
     </row>
-    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -7525,12 +7635,12 @@
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="104" t="s">
-        <v>145</v>
+      <c r="I7" s="25" t="s">
+        <v>140</v>
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="24" t="s">
         <v>44</v>
       </c>
       <c r="M7" s="24" t="s">
@@ -7546,7 +7656,7 @@
         <v>44</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="R7" s="28"/>
       <c r="S7" s="29"/>
@@ -7555,7 +7665,7 @@
     </row>
     <row r="8" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>12</v>
@@ -7587,19 +7697,19 @@
         <v>44</v>
       </c>
       <c r="Q8" s="25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R8" s="28"/>
       <c r="S8" s="29"/>
       <c r="T8" s="30"/>
       <c r="U8" s="31"/>
     </row>
-    <row r="9" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
@@ -7608,7 +7718,7 @@
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
       <c r="I9" s="25" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="26"/>
@@ -7616,7 +7726,7 @@
         <v>44</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N9" s="24" t="s">
         <v>43</v>
@@ -7628,7 +7738,7 @@
         <v>44</v>
       </c>
       <c r="Q9" s="25" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="R9" s="28"/>
       <c r="S9" s="29"/>
@@ -7637,23 +7747,19 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="24">
-        <v>1</v>
-      </c>
-      <c r="D10" s="24">
-        <v>200</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
       <c r="I10" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J10" s="24"/>
       <c r="K10" s="26"/>
@@ -7682,10 +7788,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -7693,307 +7799,268 @@
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
-      <c r="I11" s="25" t="s">
-        <v>150</v>
-      </c>
+      <c r="I11" s="24"/>
       <c r="J11" s="24"/>
       <c r="K11" s="26"/>
-      <c r="L11" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="M11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="O11" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="P11" s="24" t="s">
-        <v>44</v>
-      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
       <c r="Q11" s="25" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="R11" s="28"/>
       <c r="S11" s="29"/>
       <c r="T11" s="30"/>
       <c r="U11" s="31"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="31"/>
-    </row>
-    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="56"/>
+    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="56"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="90" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="87" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+      <c r="A14" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B14" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C14" s="34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="99" t="s">
+    <row r="15" spans="1:21" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="94" t="s">
+      <c r="B15" s="97" t="s">
         <v>130</v>
       </c>
+      <c r="C15" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="103"/>
+      <c r="B16" s="98"/>
       <c r="C16" s="35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="100"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="35" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="77"/>
+      <c r="C18" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
+      <c r="K18" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="L18" s="77"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="77"/>
+      <c r="O18" s="77"/>
+      <c r="P18" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q18" s="77"/>
+      <c r="R18" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="S18" s="78"/>
+    </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74" t="s">
+      <c r="A19" s="94"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="L19" s="74"/>
-      <c r="M19" s="74"/>
-      <c r="N19" s="74"/>
-      <c r="O19" s="74"/>
-      <c r="P19" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q19" s="74"/>
-      <c r="R19" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="S19" s="75"/>
+      <c r="K19" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="79"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="79"/>
+      <c r="P19" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q19" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="R19" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="S19" s="37" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="91"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="J20" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="L20" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="M20" s="76"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q20" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="R20" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="S20" s="37" t="s">
-        <v>62</v>
-      </c>
+      <c r="A20" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="81"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="82"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="38"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="77" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="38"/>
+      <c r="A21" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="84"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="44"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="80" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="44"/>
+      <c r="A22" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="70"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="49"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="50"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="67"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="69"/>
-      <c r="O23" s="69"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="49"/>
-      <c r="R23" s="49"/>
-      <c r="S23" s="50"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="70" t="s">
+      <c r="A23" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="73"/>
-      <c r="N24" s="73"/>
-      <c r="O24" s="73"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="54"/>
-      <c r="S24" s="55"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="76"/>
+      <c r="O23" s="76"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="R18:S18"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:G19"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:O18"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:O19"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C22:G22"/>
     <mergeCell ref="L22:O22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{87E5FC51-2E20-487C-809E-702D72E38ACE}"/>
-    <hyperlink ref="I24" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{9A04E92F-1529-4FD3-8E93-A1013850ECEB}"/>
+    <hyperlink ref="I23" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{9A04E92F-1529-4FD3-8E93-A1013850ECEB}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{BE5BBDEB-D136-4A69-B76E-B9EE18B4AADF}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{D01A25A8-47B1-4A34-B537-75FC9B240CD7}"/>
     <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{92F40FB2-A95D-48A6-9D44-842275D8A002}"/>
-    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C0E8065D-3D44-47C0-B62D-9C1975E78394}"/>
-    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{87B8DA9D-DFC9-46D8-BA58-B9DFB0075785}"/>
-    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{5FAE9D83-2CFB-4516-8C0E-0483F9E7D414}"/>
+    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{C0E8065D-3D44-47C0-B62D-9C1975E78394}"/>
+    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{87B8DA9D-DFC9-46D8-BA58-B9DFB0075785}"/>
+    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{5FAE9D83-2CFB-4516-8C0E-0483F9E7D414}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{CDA72146-A8A4-4D15-95BA-54212217969C}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{FA8306A6-9560-44AE-8D58-CD1ED4D8F35F}"/>
-    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{5ABA868F-0891-4351-9AEE-F3E42FC356A3}"/>
-    <hyperlink ref="C17" location="TipoZonaComun!A5" display="identificador" xr:uid="{E10B65B9-BDA7-4627-9804-7F151D49B328}"/>
-    <hyperlink ref="C16" location="TipoZonaComun!A5" display="identificador" xr:uid="{031EE333-7435-4C47-B98E-7785412C28EE}"/>
+    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{5ABA868F-0891-4351-9AEE-F3E42FC356A3}"/>
+    <hyperlink ref="C16" location="TipoZonaComun!A5" display="identificador" xr:uid="{E10B65B9-BDA7-4627-9804-7F151D49B328}"/>
+    <hyperlink ref="C15" location="TipoZonaComun!A5" display="identificador" xr:uid="{031EE333-7435-4C47-B98E-7785412C28EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8004,7 +8071,7 @@
           <x14:formula1>
             <xm:f>Valores!$A$7:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B11</xm:sqref>
+          <xm:sqref>B5:B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8016,7 +8083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B28FCEC-48B2-4101-A999-B6D0BE7ECE06}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView topLeftCell="I3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -8048,73 +8115,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="85" t="str">
+      <c r="B2" s="88" t="str">
         <f>'Listado Objetos de Dominio'!A8</f>
         <v>Publicación</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="86" t="str">
+      <c r="B3" s="89" t="str">
         <f>'Listado Objetos de Dominio'!B8</f>
         <v xml:space="preserve"> Objeto de dominio que representa el medio de comunicación que hay frente de publicar alguna eventualidad.</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
@@ -8396,11 +8463,11 @@
       <c r="D10" s="56"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="89"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
@@ -8414,63 +8481,63 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="97" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="101" t="s">
+      <c r="C13" s="104" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="100"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="102"/>
+      <c r="A14" s="103"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="105"/>
     </row>
     <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74" t="s">
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74" t="s">
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74" t="s">
+      <c r="L16" s="77"/>
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74" t="s">
+      <c r="Q16" s="77"/>
+      <c r="R16" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="S16" s="75"/>
+      <c r="S16" s="78"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="91"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
       <c r="H17" s="36" t="s">
         <v>58</v>
       </c>
@@ -8483,12 +8550,12 @@
       <c r="K17" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="76" t="s">
+      <c r="L17" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="79"/>
       <c r="P17" s="36" t="s">
         <v>60</v>
       </c>
@@ -8503,92 +8570,92 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
       <c r="H18" s="14"/>
       <c r="I18" s="12"/>
       <c r="J18" s="13"/>
       <c r="K18" s="12"/>
-      <c r="L18" s="79"/>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
-      <c r="O18" s="79"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="82"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
       <c r="S18" s="38"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
       <c r="H19" s="41"/>
       <c r="I19" s="39"/>
       <c r="J19" s="40"/>
       <c r="K19" s="42"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="83"/>
-      <c r="O19" s="83"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="86"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="43"/>
       <c r="R19" s="43"/>
       <c r="S19" s="44"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="46"/>
       <c r="I20" s="47"/>
       <c r="J20" s="45"/>
       <c r="K20" s="48"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
+      <c r="N20" s="72"/>
+      <c r="O20" s="72"/>
       <c r="P20" s="30"/>
       <c r="Q20" s="49"/>
       <c r="R20" s="49"/>
       <c r="S20" s="50"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
       <c r="H21" s="52"/>
       <c r="I21" s="53"/>
       <c r="J21" s="51"/>
       <c r="K21" s="52"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="73"/>
-      <c r="O21" s="73"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
+      <c r="O21" s="76"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="54"/>
       <c r="R21" s="54"/>
@@ -8596,7 +8663,7 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="L18:O18"/>
     <mergeCell ref="R16:S16"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:Q2"/>
@@ -8606,10 +8673,6 @@
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="L21:O21"/>
@@ -8622,6 +8685,10 @@
     <mergeCell ref="L19:O19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:G20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{928D26AE-809F-43A3-A6BF-D75E5E6D66DA}"/>

</xml_diff>